<commit_message>
diff excel add rows
</commit_message>
<xml_diff>
--- a/docs/sample.xlsx
+++ b/docs/sample.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>日付</t>
   </si>
@@ -89,6 +89,18 @@
   </si>
   <si>
     <t>コーヒーシュガー</t>
+  </si>
+  <si>
+    <t>Colonbia Willa</t>
+  </si>
+  <si>
+    <t>ふつう</t>
+  </si>
+  <si>
+    <t>ユニーク</t>
+  </si>
+  <si>
+    <t>キビ砂糖</t>
   </si>
 </sst>
 </file>
@@ -98,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -112,6 +124,11 @@
     </font>
     <font>
       <color theme="1"/>
+      <name val="&quot;Comic Sans MS&quot;"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FFFF00FF"/>
       <name val="&quot;Comic Sans MS&quot;"/>
     </font>
   </fonts>
@@ -135,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -152,6 +169,15 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -370,18 +396,19 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.0"/>
+    <col customWidth="1" min="1" max="1" width="12.38"/>
     <col customWidth="1" min="2" max="2" width="19.25"/>
     <col customWidth="1" min="3" max="3" width="9.5"/>
     <col customWidth="1" min="4" max="4" width="6.88"/>
     <col customWidth="1" min="5" max="5" width="10.13"/>
     <col customWidth="1" min="6" max="6" width="11.75"/>
-    <col customWidth="1" min="7" max="8" width="12.63"/>
+    <col customWidth="1" min="7" max="7" width="11.63"/>
+    <col customWidth="1" min="8" max="8" width="12.63"/>
     <col customWidth="1" min="9" max="9" width="9.75"/>
     <col customWidth="1" min="10" max="10" width="11.25"/>
     <col customWidth="1" min="11" max="11" width="11.0"/>
     <col customWidth="1" min="12" max="12" width="11.38"/>
-    <col customWidth="1" min="13" max="13" width="11.0"/>
+    <col customWidth="1" min="13" max="13" width="19.38"/>
     <col customWidth="1" min="14" max="14" width="10.5"/>
   </cols>
   <sheetData>
@@ -536,7 +563,7 @@
       <c r="F4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>13.0</v>
       </c>
       <c r="H4" s="5">
@@ -558,6 +585,50 @@
         <v>25</v>
       </c>
       <c r="N4" s="5">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6">
+        <v>44962.0</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="7">
+        <v>12.0</v>
+      </c>
+      <c r="H5" s="8">
+        <v>10.0</v>
+      </c>
+      <c r="I5" s="7">
+        <v>100.0</v>
+      </c>
+      <c r="J5" s="7">
+        <v>92.0</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="7">
+        <v>100.0</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" s="8">
         <v>5.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
diff excel delete rows
</commit_message>
<xml_diff>
--- a/docs/sample.xlsx
+++ b/docs/sample.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>日付</t>
   </si>
@@ -77,18 +77,6 @@
   </si>
   <si>
     <t>Nicaragua</t>
-  </si>
-  <si>
-    <t>Brazile Italo Disco</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>よつ葉牛乳</t>
-  </si>
-  <si>
-    <t>コーヒーシュガー</t>
   </si>
 </sst>
 </file>
@@ -98,7 +86,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -112,6 +100,11 @@
     </font>
     <font>
       <color theme="1"/>
+      <name val="&quot;Comic Sans MS&quot;"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FFFF00FF"/>
       <name val="&quot;Comic Sans MS&quot;"/>
     </font>
   </fonts>
@@ -135,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -152,6 +145,9 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -370,18 +366,19 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="10.0"/>
+    <col customWidth="1" min="1" max="1" width="12.38"/>
     <col customWidth="1" min="2" max="2" width="19.25"/>
     <col customWidth="1" min="3" max="3" width="9.5"/>
     <col customWidth="1" min="4" max="4" width="6.88"/>
     <col customWidth="1" min="5" max="5" width="10.13"/>
     <col customWidth="1" min="6" max="6" width="11.75"/>
-    <col customWidth="1" min="7" max="8" width="12.63"/>
+    <col customWidth="1" min="7" max="7" width="11.63"/>
+    <col customWidth="1" min="8" max="8" width="12.63"/>
     <col customWidth="1" min="9" max="9" width="9.75"/>
     <col customWidth="1" min="10" max="10" width="11.25"/>
     <col customWidth="1" min="11" max="11" width="11.0"/>
     <col customWidth="1" min="12" max="12" width="11.38"/>
-    <col customWidth="1" min="13" max="13" width="11.0"/>
+    <col customWidth="1" min="13" max="13" width="19.38"/>
     <col customWidth="1" min="14" max="14" width="10.5"/>
   </cols>
   <sheetData>
@@ -518,48 +515,20 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3">
-        <v>44884.0</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="5">
-        <v>13.0</v>
-      </c>
-      <c r="H4" s="5">
-        <v>10.0</v>
-      </c>
-      <c r="I4" s="5">
-        <v>80.0</v>
-      </c>
-      <c r="J4" s="5">
-        <v>94.0</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="5">
-        <v>100.0</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" s="5">
-        <v>5.0</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
     </row>
   </sheetData>
   <dataValidations>
@@ -572,7 +541,7 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E2:E4">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C4">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C2:C3">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>